<commit_message>
DOING TASK2 - 522
</commit_message>
<xml_diff>
--- a/TERM4/T4B1-ICTICT522-Evaluate_vendor_products_and_equipment/2-assessments/Vendors-Analysis.xlsx
+++ b/TERM4/T4B1-ICTICT522-Evaluate_vendor_products_and_equipment/2-assessments/Vendors-Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\Assessments\TERM4\T4B1-ICTICT522-Evaluate_vendor_products_and_equipment\2-assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE855F45-02CB-4251-9994-26FFDF0448A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D26F27-637C-4E27-B6FB-70CCC9EFAF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ABBEF023-E904-4281-9568-1F5D6C76FDD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{ABBEF023-E904-4281-9568-1F5D6C76FDD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud-S" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
   <si>
     <t>Business Base Storage</t>
   </si>
@@ -198,6 +198,126 @@
   </si>
   <si>
     <t>Business Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VENDOR - Router  </t>
+  </si>
+  <si>
+    <t>VENDOR - Switch</t>
+  </si>
+  <si>
+    <t>VENDOR - Cables</t>
+  </si>
+  <si>
+    <t>VENDOR - Wi-Fi Modem</t>
+  </si>
+  <si>
+    <t>router compatibility protocols</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>Symmetry</t>
+  </si>
+  <si>
+    <t>Access Technology</t>
+  </si>
+  <si>
+    <t>Symmetrical Bandwidth</t>
+  </si>
+  <si>
+    <t>Contention Ratio</t>
+  </si>
+  <si>
+    <t>Network Segmentation</t>
+  </si>
+  <si>
+    <t>Static IP Addressing</t>
+  </si>
+  <si>
+    <t>Fault Restoration Target</t>
+  </si>
+  <si>
+    <t>Failover / Redundancy</t>
+  </si>
+  <si>
+    <t>WAN Port Throughput Capacity</t>
+  </si>
+  <si>
+    <t>NAT and Firewall Processing Throughput</t>
+  </si>
+  <si>
+    <t>QoS and Traffic Shaping Capability</t>
+  </si>
+  <si>
+    <t>Multiple SSID to VLAN Mapping</t>
+  </si>
+  <si>
+    <t>Integrated Captive Portal Functionality</t>
+  </si>
+  <si>
+    <t>Layer 2 or Layer 3 Managed Switch Capability</t>
+  </si>
+  <si>
+    <t>SFP/SFP+ Uplink Ports for Router Connection</t>
+  </si>
+  <si>
+    <t>Quality of Service (QoS) Implementation</t>
+  </si>
+  <si>
+    <t>Remote Management and Monitoring Features</t>
+  </si>
+  <si>
+    <t>Enterprise Grade Security Features</t>
+  </si>
+  <si>
+    <t>Wi-Fi Standard</t>
+  </si>
+  <si>
+    <t>VPN Gateway Functionality</t>
+  </si>
+  <si>
+    <t>DHCP and Concurrent Session Management</t>
+  </si>
+  <si>
+    <t>Standards Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Backplane Switching Capacity </t>
+  </si>
+  <si>
+    <t>VLAN Support  and Port Isolation</t>
+  </si>
+  <si>
+    <t>Wired Enterprise Access Point Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gigabit Ethernet Port Density</t>
+  </si>
+  <si>
+    <t>Cable Category</t>
+  </si>
+  <si>
+    <t>Shielding Type</t>
+  </si>
+  <si>
+    <t>PoE Compatibility and Thermal Stability</t>
+  </si>
+  <si>
+    <t>10 Gigabit Ethernet Support</t>
+  </si>
+  <si>
+    <t>Pure Copper Conductors</t>
+  </si>
+  <si>
+    <t>Australian Standards Compliance</t>
+  </si>
+  <si>
+    <t>Certified Installation and Testing Requirements</t>
   </si>
 </sst>
 </file>
@@ -289,19 +409,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -311,9 +425,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -326,14 +437,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,7 +786,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE309197-8BCE-4D3F-A681-8473C7992CFF}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
@@ -677,319 +794,177 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="8.88671875" style="3"/>
-    <col min="9" max="9" width="10.88671875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="3" customWidth="1"/>
-    <col min="12" max="14" width="8.88671875" style="3"/>
-    <col min="15" max="15" width="14.77734375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11.77734375" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="10.88671875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="2" customWidth="1"/>
+    <col min="12" max="14" width="8.88671875" style="2"/>
+    <col min="15" max="15" width="14.77734375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="72" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="6" spans="1:16" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -999,67 +974,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9BB152-C575-441E-85DE-E365BB70FAC5}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="2" max="3" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1072,9 +1050,10 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1087,6 +1066,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1095,12 +1075,412 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FF507-883C-4859-82B8-ECE60BC719EF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+    </row>
+    <row r="5" spans="1:17" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+    </row>
+    <row r="9" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+    </row>
+    <row r="10" spans="1:17" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+    </row>
+    <row r="14" spans="1:17" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1121,84 +1501,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>